<commit_message>
Fix bugs accessing GBIF, improve output
</commit_message>
<xml_diff>
--- a/Config/DatabaseInfo.xlsx
+++ b/Config/DatabaseInfo.xlsx
@@ -86,6 +86,48 @@
     <t xml:space="preserve">Group; Code</t>
   </si>
   <si>
+    <t xml:space="preserve">GloNAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxon_x_List_GloNAF_withcountrynames.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vascular plants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standardized_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstRecords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlobalAlienSpeciesFirstRecordDatabase_v1.2_withcountries.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PresentStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstRecord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LifeForm; FirstRecord_orig</t>
+  </si>
+  <si>
     <t xml:space="preserve">GAVIA</t>
   </si>
   <si>
@@ -96,48 +138,6 @@
   </si>
   <si>
     <t xml:space="preserve">CountryName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FirstRecords</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GlobalAlienSpeciesFirstRecordDatabase_v1.2_withcountries.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PresentStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FirstRecord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LifeForm; FirstRecord_orig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GloNAF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxon_x_List_GloNAF_withcountrynames.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vascular plants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standardized_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status</t>
   </si>
   <si>
     <t xml:space="preserve">GRIIS</t>
@@ -279,19 +279,19 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="12.5561224489796"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="39.1479591836735"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
@@ -373,58 +373,58 @@
         <v>23</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="0" t="s">
         <v>38</v>
       </c>
     </row>
@@ -436,7 +436,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>41</v>
@@ -445,7 +445,7 @@
         <v>42</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>43</v>
@@ -481,14 +481,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="12.5561224489796"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="39.1479591836735"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
@@ -561,68 +561,68 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,7 +633,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>41</v>
@@ -642,7 +642,7 @@
         <v>42</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Allow sub-species levels; minor modifications
</commit_message>
<xml_diff>
--- a/Config/DatabaseInfo.xlsx
+++ b/Config/DatabaseInfo.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t xml:space="preserve">Dataset_brief_name</t>
   </si>
@@ -32,145 +32,151 @@
     <t xml:space="preserve">Taxon_group</t>
   </si>
   <si>
+    <t xml:space="preserve">Column_taxon_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column_scientificName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column_author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column_kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column_region_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column_country_ISO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column_island_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column_first_record1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column_first_record2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column_additional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAVIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAVIA_main_data_table.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binomial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CountryName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IntroducedDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstRecords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlobalAlienSpeciesFirstRecordDatabase_v1.2_withcountries.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PresentStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstRecord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LifeForm; FirstRecord_orig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AmphRep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AmphibiansReptiles_Capinha-etal2017.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amphibians; Reptiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GloNAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxon_x_List_GloNAF_withcountrynames.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vascular plants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standardized_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRIIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRIIS_sTwist_Hanno_Aug92019_resend.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scientificName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">countryCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolved date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habitat; establishmentMeans; IsInvasive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_countrynames</t>
+  </si>
+  <si>
     <t xml:space="preserve">Column_species_name</t>
   </si>
   <si>
-    <t xml:space="preserve">Column_scientificName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column_author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column_kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column_region_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column_country_ISO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column_island_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column_status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column_first_record1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column_first_record2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column_additional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAVIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAVIA_main_data_table.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Binomial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CountryName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IntroducedDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FirstRecords</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GlobalAlienSpeciesFirstRecordDatabase_v1.2_withcountries.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PresentStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FirstRecord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LifeForm; FirstRecord_orig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AmphRep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AmphibiansReptiles_Capinha-etal2017.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amphibians; Reptiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species</t>
+    <t xml:space="preserve">ReplaceCountryNames_AmphRep.r</t>
   </si>
   <si>
     <t xml:space="preserve">Group; Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GloNAF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxon_x_List_GloNAF_withcountrynames.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vascular plants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standardized_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRIIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRIIS_sTwist_Hanno_Aug92019_resend.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scientificName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">countryCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolved date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">habitat; establishmentMeans; IsInvasive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R_countrynames</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReplaceCountryNames_AmphRep.r</t>
   </si>
   <si>
     <t xml:space="preserve">GAVIA_NaturalSpecCountry.xlsx</t>
@@ -280,23 +286,23 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -340,7 +346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>14</v>
       </c>
@@ -360,7 +366,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>20</v>
       </c>
@@ -386,7 +392,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>28</v>
       </c>
@@ -406,7 +412,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>33</v>
       </c>
@@ -429,7 +435,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>40</v>
       </c>
@@ -485,15 +491,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,7 +516,7 @@
         <v>48</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>4</v>
@@ -551,7 +557,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>31</v>
@@ -560,7 +566,7 @@
         <v>24</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +574,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>16</v>
@@ -634,7 +640,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>22</v>
@@ -655,7 +661,7 @@
         <v>46</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix import of files from intermediate folder
Files are now identified by exact matches of full name rather than parts of file name
</commit_message>
<xml_diff>
--- a/Config/DatabaseInfo.xlsx
+++ b/Config/DatabaseInfo.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
   <si>
     <t xml:space="preserve">Dataset_brief_name</t>
   </si>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">AmphRep</t>
   </si>
   <si>
-    <t xml:space="preserve">AmphibiansReptiles_Capinha-etal2017_example.xlsx</t>
+    <t xml:space="preserve">AmphibiansReptiles_Capinha-etal2017.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">Amphibians; Reptiles</t>
@@ -104,7 +104,7 @@
     <t xml:space="preserve">GAVIA</t>
   </si>
   <si>
-    <t xml:space="preserve">GAVIA_taxon_region_list_example.xlsx</t>
+    <t xml:space="preserve">GAVIA_taxon_region_list.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">Birds</t>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">GRIIS</t>
   </si>
   <si>
-    <t xml:space="preserve">GRIIS_sTwist_Hanno_Aug92019_resend_example.xlsx</t>
+    <t xml:space="preserve">GRIIS_sTwist_Hanno_Aug92019_resend.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">All</t>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">countryCode</t>
   </si>
   <si>
-    <t xml:space="preserve">Resolved date</t>
+    <t xml:space="preserve">Resolved.date</t>
   </si>
   <si>
     <t xml:space="preserve">establishmentMeans</t>
@@ -170,7 +170,7 @@
     <t xml:space="preserve">GloNAF</t>
   </si>
   <si>
-    <t xml:space="preserve">GloNAF_taxon_region_list_example.xlsx</t>
+    <t xml:space="preserve">GloNAF_taxon_region_list.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">Vascular plants</t>
@@ -188,7 +188,7 @@
     <t xml:space="preserve">FirstRecords</t>
   </si>
   <si>
-    <t xml:space="preserve">GlobalAlienSpeciesFirstRecordDatabase_v1.2_withcountries_example.xlsx</t>
+    <t xml:space="preserve">GlobalAlienSpeciesFirstRecordDatabase_v1.2_withcountries.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">Taxon</t>
@@ -206,25 +206,10 @@
     <t xml:space="preserve">FirstRecord_orig</t>
   </si>
   <si>
-    <t xml:space="preserve">AmphibiansReptiles_Capinha-etal2017.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAVIA_taxon_region_list.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRIIS_sTwist_Hanno_Aug92019_resend.xlsx</t>
-  </si>
-  <si>
     <t xml:space="preserve">Introduced_before (year)</t>
   </si>
   <si>
     <t xml:space="preserve">Introduced_after (year)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GloNAF_taxon_region_list.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GlobalAlienSpeciesFirstRecordDatabase_v1.2_withcountries.xlsx</t>
   </si>
 </sst>
 </file>
@@ -337,9 +322,9 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topRight" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -482,7 +467,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>36</v>
       </c>
@@ -618,7 +603,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>21</v>
@@ -641,7 +626,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>28</v>
@@ -679,7 +664,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>38</v>
@@ -700,10 +685,10 @@
         <v>43</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O3" s="0" t="s">
         <v>45</v>
@@ -720,7 +705,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>50</v>
@@ -743,7 +728,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>38</v>

</xml_diff>